<commit_message>
adding new mapping from Simon and receiving two new versions from Josh
</commit_message>
<xml_diff>
--- a/DnaRepairSpreadsheetParser/test/exampleData/postUploadProcessing/post-processing.xlsx
+++ b/DnaRepairSpreadsheetParser/test/exampleData/postUploadProcessing/post-processing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>attribue_id</t>
   </si>
@@ -30,9 +30,6 @@
     <t>ad_id</t>
   </si>
   <si>
-    <t>assay component role</t>
-  </si>
-  <si>
     <t>Source Context</t>
   </si>
   <si>
@@ -45,19 +42,37 @@
     <t>New_AssayContext_group</t>
   </si>
   <si>
-    <t>assay protocol</t>
-  </si>
-  <si>
-    <t>cell cycle assay</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>assay design</t>
-  </si>
-  <si>
-    <t>cell-based format</t>
+    <t xml:space="preserve">  504727</t>
+  </si>
+  <si>
+    <t>purified Salmon sperm DNA</t>
+  </si>
+  <si>
+    <t>biological role</t>
+  </si>
+  <si>
+    <t>assay component type</t>
+  </si>
+  <si>
+    <t>purified DNA</t>
+  </si>
+  <si>
+    <t>species name</t>
+  </si>
+  <si>
+    <t>Salmo salar</t>
+  </si>
+  <si>
+    <t>biological tissue</t>
+  </si>
+  <si>
+    <t>sperm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  588364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  463198</t>
   </si>
 </sst>
 </file>
@@ -415,32 +430,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C9" sqref="C9:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -450,7 +465,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -465,27 +480,24 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>32</v>
-      </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -493,12 +505,107 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="b">
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>